<commit_message>
implemented grid search in abm
</commit_message>
<xml_diff>
--- a/notebooks/abm_calibration_results.xlsx
+++ b/notebooks/abm_calibration_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,28 +517,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99.9744403644487</v>
+        <v>589.5073219971033</v>
       </c>
       <c r="C3" t="n">
-        <v>199.4604323684837</v>
+        <v>118.3377088749102</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1094939215928832</v>
+        <v>-0.2525405932891465</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1976230079612077</v>
+        <v>0.1792744057164483</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -549,28 +549,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>151.116759415841</v>
+        <v>519.6009647262586</v>
       </c>
       <c r="C4" t="n">
-        <v>83.15333067786906</v>
+        <v>187.7976198069879</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.1322868249172909</v>
+        <v>-0.2377709314083304</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04514426263484212</v>
+        <v>0.3609646339632479</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
@@ -581,31 +581,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>402.8981992298889</v>
+        <v>888.508971551362</v>
       </c>
       <c r="C5" t="n">
-        <v>13.46246124012389</v>
+        <v>101.1037639479126</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2103283418938891</v>
+        <v>-0.3078833134696223</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2358607796743009</v>
+        <v>0.2860351276956745</v>
       </c>
       <c r="F5" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -613,31 +613,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>393.490193571921</v>
+        <v>242.6967980106479</v>
       </c>
       <c r="C6" t="n">
-        <v>13.76160431670547</v>
+        <v>170.3184075495041</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2079487273241885</v>
+        <v>-0.165484481028648</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1843612838902526</v>
+        <v>0.2869223698400488</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -645,31 +645,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>10.89191387648743</v>
+        <v>680.2996950347989</v>
       </c>
       <c r="C7" t="n">
-        <v>218.5407040862787</v>
+        <v>381.3802935565604</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.04123298062061823</v>
+        <v>-0.2707236054680359</v>
       </c>
       <c r="E7" t="n">
-        <v>0.06395215562991183</v>
+        <v>0.3351760706052715</v>
       </c>
       <c r="F7" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
         <v>5</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -677,31 +677,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>358.5786590728679</v>
+        <v>523.8877370676529</v>
       </c>
       <c r="C8" t="n">
-        <v>51.2369696558343</v>
+        <v>22.0878045005566</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1989669058228524</v>
+        <v>-0.2385636810105169</v>
       </c>
       <c r="E8" t="n">
-        <v>0.182935937063725</v>
+        <v>0.2904531453183771</v>
       </c>
       <c r="F8" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -709,31 +709,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>791.7773956520663</v>
+        <v>1711.378493414712</v>
       </c>
       <c r="C9" t="n">
-        <v>132.523925221364</v>
+        <v>14.59958992115568</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.2912073026988312</v>
+        <v>-0.4235182872253599</v>
       </c>
       <c r="E9" t="n">
-        <v>0.3310771092092178</v>
+        <v>0.3758699848913475</v>
       </c>
       <c r="F9" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -741,31 +741,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>328.5435742681925</v>
+        <v>566.4993376159734</v>
       </c>
       <c r="C10" t="n">
-        <v>26.73657211966537</v>
+        <v>329.3514114009142</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1908283559213509</v>
+        <v>-0.2478306273264488</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2138123717257993</v>
+        <v>0.1191269094380362</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -773,31 +773,31 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>392.0280490912139</v>
+        <v>210.4459512179345</v>
       </c>
       <c r="C11" t="n">
-        <v>64.91169834706055</v>
+        <v>451.8906391176505</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.2076262376725438</v>
+        <v>-0.1547643703814152</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1632145451626222</v>
+        <v>0.07694179851055039</v>
       </c>
       <c r="F11" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -805,31 +805,31 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>237.4474526203753</v>
+        <v>931.6156784792616</v>
       </c>
       <c r="C12" t="n">
-        <v>287.5168343681967</v>
+        <v>129.2722209442764</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.1637992841579815</v>
+        <v>-0.3150426600678212</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1290458190201539</v>
+        <v>0.2571791026877445</v>
       </c>
       <c r="F12" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" t="n">
         <v>5</v>
-      </c>
-      <c r="I12" t="n">
-        <v>5</v>
-      </c>
-      <c r="J12" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -837,28 +837,28 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>307.6000535573008</v>
+        <v>2321.020196042473</v>
       </c>
       <c r="C13" t="n">
-        <v>57.87965418740833</v>
+        <v>23.07125353896587</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.1849534395192915</v>
+        <v>-0.4916350421458058</v>
       </c>
       <c r="E13" t="n">
-        <v>0.1506852401810309</v>
+        <v>0.4394196756377313</v>
       </c>
       <c r="F13" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
@@ -869,31 +869,1567 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>157.8975582341676</v>
+        <v>1121.552090873373</v>
       </c>
       <c r="C14" t="n">
-        <v>252.5640496409812</v>
+        <v>152.4356373341663</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.1352432113843841</v>
+        <v>-0.3447282416447004</v>
       </c>
       <c r="E14" t="n">
-        <v>0.08084761718719043</v>
+        <v>0.191335136514745</v>
       </c>
       <c r="F14" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>3</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>852.8493278259953</v>
+      </c>
+      <c r="C15" t="n">
+        <v>272.7105318362577</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.3019123750856398</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.27962428476794</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1389.704681792834</v>
+      </c>
+      <c r="C16" t="n">
+        <v>133.5202155813865</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-0.382663129115527</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.3930431992599698</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>3</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1043.658135512566</v>
+      </c>
+      <c r="C17" t="n">
+        <v>210.5278861526829</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-0.3329205329835486</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.2535319571028445</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3</v>
+      </c>
+      <c r="J17" t="n">
         <v>5</v>
       </c>
-      <c r="I14" t="n">
-        <v>10</v>
-      </c>
-      <c r="J14" t="n">
-        <v>2</v>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>827.2089051027593</v>
+      </c>
+      <c r="C18" t="n">
+        <v>574.0247392246473</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.2974757595310299</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.2166572275205575</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>4</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1756.302671572533</v>
+      </c>
+      <c r="C19" t="n">
+        <v>20.34155082666312</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.4289120477426835</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.3328239696599155</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>4</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>889.839965149197</v>
+      </c>
+      <c r="C20" t="n">
+        <v>69.38584049881301</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.3081004817559397</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.3529065199813378</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>4</v>
+      </c>
+      <c r="J20" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>686.4023218284253</v>
+      </c>
+      <c r="C21" t="n">
+        <v>167.7576027740055</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-0.2717993656689507</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.2381904583158775</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>4</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>339.0360104892509</v>
+      </c>
+      <c r="C22" t="n">
+        <v>814.1444798197695</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-0.1936997973745694</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.1443688262499098</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>4</v>
+      </c>
+      <c r="J22" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>778.8127203159804</v>
+      </c>
+      <c r="C23" t="n">
+        <v>195.368758526928</v>
+      </c>
+      <c r="D23" t="n">
+        <v>-0.2889018945173942</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.2299508596826763</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="n">
+        <v>5</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1734.118351549883</v>
+      </c>
+      <c r="C24" t="n">
+        <v>25.85698892061734</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.4262670013152521</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.3922472825085811</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>5</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>977.4201780701376</v>
+      </c>
+      <c r="C25" t="n">
+        <v>46.62001600183561</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-0.3224210083056703</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.3045337964315099</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>5</v>
+      </c>
+      <c r="J25" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1329.008576141663</v>
+      </c>
+      <c r="C26" t="n">
+        <v>13.75610391241223</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.3743519138922201</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.311264578006101</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>5</v>
+      </c>
+      <c r="J26" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1143.029915154799</v>
+      </c>
+      <c r="C27" t="n">
+        <v>47.85966785320325</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.347907494127882</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.4169180130442285</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>5</v>
+      </c>
+      <c r="J27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>104.7319230343306</v>
+      </c>
+      <c r="C28" t="n">
+        <v>346.2884738020387</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.1119710396581513</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.1861444281630721</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1334.29872365332</v>
+      </c>
+      <c r="C29" t="n">
+        <v>52.88500556629781</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-0.3751159596117742</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.4099684276436965</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>129.3772160543861</v>
+      </c>
+      <c r="C30" t="n">
+        <v>436.8625432138296</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-0.1233502985115176</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.06539481118753032</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>378.0811399335689</v>
+      </c>
+      <c r="C31" t="n">
+        <v>328.2365793256095</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-0.2042244556220173</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.1303295235502339</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>536.6039460873664</v>
+      </c>
+      <c r="C32" t="n">
+        <v>372.8679330435958</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-0.2415014217964582</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.2267837219136855</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>421.6669136322025</v>
+      </c>
+      <c r="C33" t="n">
+        <v>55.85464354894377</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-0.214984594575524</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.1792825324368781</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" t="n">
+        <v>2</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>509.4600942169862</v>
+      </c>
+      <c r="C34" t="n">
+        <v>71.62917307682318</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-0.235424117377408</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.2659832041296704</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" t="n">
+        <v>2</v>
+      </c>
+      <c r="J34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>248.9123020851561</v>
+      </c>
+      <c r="C35" t="n">
+        <v>541.5757799624081</v>
+      </c>
+      <c r="D35" t="n">
+        <v>-0.1675322148508443</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.2108522891850306</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>285.6467974081051</v>
+      </c>
+      <c r="C36" t="n">
+        <v>288.3712380306507</v>
+      </c>
+      <c r="D36" t="n">
+        <v>-0.1787437038372912</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.1300704135150779</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2</v>
+      </c>
+      <c r="I36" t="n">
+        <v>2</v>
+      </c>
+      <c r="J36" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>544.2560604089375</v>
+      </c>
+      <c r="C37" t="n">
+        <v>62.43417798134474</v>
+      </c>
+      <c r="D37" t="n">
+        <v>-0.2430048757004073</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.2602937772159372</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" t="n">
+        <v>2</v>
+      </c>
+      <c r="J37" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>343.1596060637521</v>
+      </c>
+      <c r="C38" t="n">
+        <v>98.42042476711757</v>
+      </c>
+      <c r="D38" t="n">
+        <v>-0.1948856811014922</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.1686566852660646</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" t="n">
+        <v>3</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>723.4804715024706</v>
+      </c>
+      <c r="C39" t="n">
+        <v>9.274213321659087</v>
+      </c>
+      <c r="D39" t="n">
+        <v>-0.2786895610934736</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.2841883533870563</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I39" t="n">
+        <v>3</v>
+      </c>
+      <c r="J39" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>698.9090854338259</v>
+      </c>
+      <c r="C40" t="n">
+        <v>193.2419758974525</v>
+      </c>
+      <c r="D40" t="n">
+        <v>-0.2741971309119228</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.2659731115710186</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2</v>
+      </c>
+      <c r="I40" t="n">
+        <v>3</v>
+      </c>
+      <c r="J40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>52.51118419817914</v>
+      </c>
+      <c r="C41" t="n">
+        <v>708.11820117806</v>
+      </c>
+      <c r="D41" t="n">
+        <v>-0.08138931448453653</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-0.07195972621278539</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" t="n">
+        <v>3</v>
+      </c>
+      <c r="J41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>907.180021964779</v>
+      </c>
+      <c r="C42" t="n">
+        <v>15.37240663523016</v>
+      </c>
+      <c r="D42" t="n">
+        <v>-0.3109544624007848</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.3392395779641633</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" t="n">
+        <v>2</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3</v>
+      </c>
+      <c r="J42" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>389.9091970964738</v>
+      </c>
+      <c r="C43" t="n">
+        <v>86.827267183659</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-0.2070840972008504</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.09260805811808559</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43" t="n">
+        <v>4</v>
+      </c>
+      <c r="J43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>774.3603406683168</v>
+      </c>
+      <c r="C44" t="n">
+        <v>55.17019426436505</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-0.2880187376603104</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.2274660483889071</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H44" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" t="n">
+        <v>4</v>
+      </c>
+      <c r="J44" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>129.238620039313</v>
+      </c>
+      <c r="C45" t="n">
+        <v>243.1106926485203</v>
+      </c>
+      <c r="D45" t="n">
+        <v>-0.1231555288490083</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.005463624743983729</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1</v>
+      </c>
+      <c r="H45" t="n">
+        <v>2</v>
+      </c>
+      <c r="I45" t="n">
+        <v>4</v>
+      </c>
+      <c r="J45" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>309.5218199202319</v>
+      </c>
+      <c r="C46" t="n">
+        <v>24.35329843234646</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-0.1854289409699432</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.07494047977518921</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1</v>
+      </c>
+      <c r="H46" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" t="n">
+        <v>4</v>
+      </c>
+      <c r="J46" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>252.1354803226579</v>
+      </c>
+      <c r="C47" t="n">
+        <v>386.1801723707599</v>
+      </c>
+      <c r="D47" t="n">
+        <v>-0.1685140933937601</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.08824056004517275</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I47" t="n">
+        <v>4</v>
+      </c>
+      <c r="J47" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>361.8210106859125</v>
+      </c>
+      <c r="C48" t="n">
+        <v>888.3125044169261</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-0.1997389219979468</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.2206089794082836</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" t="n">
+        <v>2</v>
+      </c>
+      <c r="I48" t="n">
+        <v>5</v>
+      </c>
+      <c r="J48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>214.2706631773327</v>
+      </c>
+      <c r="C49" t="n">
+        <v>743.4842100393103</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-0.1558654115420938</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.02051637621376246</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2</v>
+      </c>
+      <c r="I49" t="n">
+        <v>5</v>
+      </c>
+      <c r="J49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>441.4440467940825</v>
+      </c>
+      <c r="C50" t="n">
+        <v>189.7102043780105</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-0.2198350453167091</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.109741931601688</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I50" t="n">
+        <v>5</v>
+      </c>
+      <c r="J50" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>224.67947720511</v>
+      </c>
+      <c r="C51" t="n">
+        <v>78.40303789190882</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-0.1593408071696373</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.009139620047806753</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2</v>
+      </c>
+      <c r="I51" t="n">
+        <v>5</v>
+      </c>
+      <c r="J51" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>468.6473801521736</v>
+      </c>
+      <c r="C52" t="n">
+        <v>342.2171893531855</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-0.2263253187899773</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.2399827243713688</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" t="n">
+        <v>2</v>
+      </c>
+      <c r="I52" t="n">
+        <v>5</v>
+      </c>
+      <c r="J52" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>86.61870226798231</v>
+      </c>
+      <c r="C53" t="n">
+        <v>376.6895857605215</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-0.102618698193712</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.1122932289228508</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3</v>
+      </c>
+      <c r="I53" t="n">
+        <v>1</v>
+      </c>
+      <c r="J53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>25.03452312677011</v>
+      </c>
+      <c r="C54" t="n">
+        <v>544.8355221446233</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-0.05905474655498338</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.06288707901109232</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3</v>
+      </c>
+      <c r="I54" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1217.857001726233</v>
+      </c>
+      <c r="C55" t="n">
+        <v>108.1393862394941</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-0.3588297098866297</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.3721372510019473</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" t="n">
+        <v>1</v>
+      </c>
+      <c r="J55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>100.6394285582988</v>
+      </c>
+      <c r="C56" t="n">
+        <v>154.1682416640006</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-0.1096222462251276</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.01018448609622913</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1</v>
+      </c>
+      <c r="H56" t="n">
+        <v>3</v>
+      </c>
+      <c r="I56" t="n">
+        <v>1</v>
+      </c>
+      <c r="J56" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>613.7016489209019</v>
+      </c>
+      <c r="C57" t="n">
+        <v>467.4409272957522</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-0.2575938651481302</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.2204007319363099</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G57" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" t="n">
+        <v>3</v>
+      </c>
+      <c r="I57" t="n">
+        <v>1</v>
+      </c>
+      <c r="J57" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>496.0656872837542</v>
+      </c>
+      <c r="C58" t="n">
+        <v>233.1108008004908</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-0.2325285264771272</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.2194185034512761</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1</v>
+      </c>
+      <c r="H58" t="n">
+        <v>3</v>
+      </c>
+      <c r="I58" t="n">
+        <v>2</v>
+      </c>
+      <c r="J58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>450.1246360484679</v>
+      </c>
+      <c r="C59" t="n">
+        <v>351.3685003537796</v>
+      </c>
+      <c r="D59" t="n">
+        <v>-0.2219659825637058</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.1292985814321041</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1</v>
+      </c>
+      <c r="H59" t="n">
+        <v>3</v>
+      </c>
+      <c r="I59" t="n">
+        <v>2</v>
+      </c>
+      <c r="J59" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>50.52268476603606</v>
+      </c>
+      <c r="C60" t="n">
+        <v>868.3923431614296</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-0.07971610866925946</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.08052752890975037</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="n">
+        <v>3</v>
+      </c>
+      <c r="I60" t="n">
+        <v>2</v>
+      </c>
+      <c r="J60" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>376.6077748791666</v>
+      </c>
+      <c r="C61" t="n">
+        <v>45.05800980734121</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-0.2036767224025918</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.1959533557147662</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G61" t="n">
+        <v>1</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3</v>
+      </c>
+      <c r="I61" t="n">
+        <v>2</v>
+      </c>
+      <c r="J61" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>125.9894882593012</v>
+      </c>
+      <c r="C62" t="n">
+        <v>366.6267690531009</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-0.1218608619645475</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.1002964111291127</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" t="n">
+        <v>3</v>
+      </c>
+      <c r="I62" t="n">
+        <v>2</v>
+      </c>
+      <c r="J62" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>